<commit_message>
Updated Agile Document Excel sheets with latest data
</commit_message>
<xml_diff>
--- a/Agile Document/Agile_Template_Filled.xlsx
+++ b/Agile Document/Agile_Template_Filled.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lavanya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\live-ai-speech-translator\Agile Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5288628-A62E-4B72-8B08-47A8EC37EE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5867EC29-7173-46E8-B987-889E74A8399A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
   <si>
     <t>Planned Sprint</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Hugging Face Transformers, GPT API</t>
   </si>
   <si>
-    <t>Team B</t>
-  </si>
-  <si>
     <t>Sprint 3</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>Memory optimization tools</t>
-  </si>
-  <si>
-    <t>Both Teams</t>
   </si>
   <si>
     <t>Planned</t>
@@ -729,7 +723,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -815,7 +809,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -823,22 +817,22 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -849,80 +843,80 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
       <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
         <v>39</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -943,93 +937,93 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
         <v>48</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>49</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
-      </c>
-      <c r="V1" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>65</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -1038,80 +1032,80 @@
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>71</v>
       </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>74</v>
-      </c>
       <c r="H3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3">
         <v>12</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>76</v>
       </c>
-      <c r="D4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>77</v>
       </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" t="s">
-        <v>79</v>
-      </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I4">
         <v>10</v>
@@ -1119,28 +1113,28 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>82</v>
       </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>84</v>
-      </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I5">
         <v>15</v>
@@ -1161,72 +1155,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>86</v>
-      </c>
-      <c r="C1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1244,106 +1238,106 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>102</v>
-      </c>
-      <c r="G1" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>106</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>107</v>
-      </c>
-      <c r="G2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" t="s">
         <v>110</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4" t="s">
         <v>114</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>115</v>
-      </c>
-      <c r="G4" t="s">
-        <v>116</v>
-      </c>
-      <c r="H4" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>